<commit_message>
Dataset more cleanup, django import-export app added for easy database population
</commit_message>
<xml_diff>
--- a/data/raw_data.xlsx
+++ b/data/raw_data.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\card\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\nsu.fall.2018.cse327.1.t2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B8FA1E-A76E-4919-B6E4-0C0FF3864CA1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA43358-0313-4A81-AC04-0A13FC653914}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2942" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2914" uniqueCount="312">
   <si>
     <t>Card Name</t>
   </si>
@@ -292,9 +292,6 @@
     <t>Prepaid</t>
   </si>
   <si>
-    <t>USD 350</t>
-  </si>
-  <si>
     <t>Brac Bank Travel Card</t>
   </si>
   <si>
@@ -331,9 +328,6 @@
     <t>https://dhakabankltd.com/credit-card/</t>
   </si>
   <si>
-    <t>5,00,000.00</t>
-  </si>
-  <si>
     <t>Dhaka Bank Debit Card</t>
   </si>
   <si>
@@ -358,9 +352,6 @@
     <t xml:space="preserve">Credit </t>
   </si>
   <si>
-    <t>20,00,000.00</t>
-  </si>
-  <si>
     <t>Dutch Bangla VISA platinum Credit Card</t>
   </si>
   <si>
@@ -382,9 +373,6 @@
     <t>https://www.dutchbanglabank.com/electronic-banking/visagoldlocalcredit.html</t>
   </si>
   <si>
-    <t>5,00,000</t>
-  </si>
-  <si>
     <t>Dutch Bangla VISA classic International Credit Card</t>
   </si>
   <si>
@@ -466,18 +454,12 @@
     <t>http://jamunabankbd.com/front/productdetails/27/87/120</t>
   </si>
   <si>
-    <t>1,00,000.00</t>
-  </si>
-  <si>
     <t>Jamuna Bank VISA Gold Credit Card</t>
   </si>
   <si>
     <t>http://jamunabankbd.com/front/productdetails/27/87/121</t>
   </si>
   <si>
-    <t>2,00,000.00</t>
-  </si>
-  <si>
     <t>Jamuna Bank VISA Dual Gold Credit Card</t>
   </si>
   <si>
@@ -505,9 +487,6 @@
     <t>https://www.meghnabank.com.bd/mbl/silver_credit_card.php</t>
   </si>
   <si>
-    <t>3,00,000.00</t>
-  </si>
-  <si>
     <t>Meghna Visa Gold Credit Card</t>
   </si>
   <si>
@@ -523,9 +502,6 @@
     <t>https://www.midlandbankbd.net/mdb-credit-card/</t>
   </si>
   <si>
-    <t>1,99,000.00</t>
-  </si>
-  <si>
     <t>MDB Visa Platinum Dual Credit Card</t>
   </si>
   <si>
@@ -583,9 +559,6 @@
     <t>http://www.mutualtrustbank.com/cards/credit-card/dual-currency-credit-card</t>
   </si>
   <si>
-    <t>1,000,00.00</t>
-  </si>
-  <si>
     <t>MTB VISA Platinum Credit Card</t>
   </si>
   <si>
@@ -745,9 +718,6 @@
     <t>https://www.primebank.com.bd/index.php/home/platinum_credit_card</t>
   </si>
   <si>
-    <t>25,00,000.00</t>
-  </si>
-  <si>
     <t>Prime Bank Hasanah Credit Card</t>
   </si>
   <si>
@@ -775,9 +745,6 @@
     <t>https://www.tblbd.com/visa-international-classic-dual</t>
   </si>
   <si>
-    <t>120,00,000.00</t>
-  </si>
-  <si>
     <t>Trust Bank Visa International Gold Card</t>
   </si>
   <si>
@@ -847,16 +814,10 @@
     <t>UCB Visa Gold Credit Card</t>
   </si>
   <si>
-    <t>2,000,00.00</t>
-  </si>
-  <si>
     <t>UCB MasterCard Gold Credit Card</t>
   </si>
   <si>
     <t>UCB Visa Platinum Credit Card</t>
-  </si>
-  <si>
-    <t>5,000,00.00</t>
   </si>
   <si>
     <t>UCB MasterCard Platinum Credit Card</t>
@@ -1417,16 +1378,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X985"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C135" sqref="C135"/>
+    <sheetView tabSelected="1" topLeftCell="D120" workbookViewId="0">
+      <selection activeCell="H140" sqref="H140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="50.5703125" customWidth="1"/>
     <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="60.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="3" max="3" width="91.5703125" customWidth="1"/>
+    <col min="4" max="4" width="41.5703125" customWidth="1"/>
     <col min="5" max="5" width="21.140625" customWidth="1"/>
     <col min="6" max="6" width="34.28515625" customWidth="1"/>
     <col min="7" max="7" width="30.28515625" customWidth="1"/>
@@ -3238,8 +3199,9 @@
       <c r="G25" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>90</v>
+      <c r="H25" s="1">
+        <f>350*80</f>
+        <v>28000</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>46</v>
@@ -3292,13 +3254,13 @@
     </row>
     <row r="26" spans="1:24" ht="15.75" customHeight="1">
       <c r="A26" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B26" t="s">
         <v>77</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>89</v>
@@ -3366,13 +3328,13 @@
     </row>
     <row r="27" spans="1:24" ht="15.75" customHeight="1">
       <c r="A27" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" t="s">
         <v>93</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>27</v>
@@ -3440,13 +3402,13 @@
     </row>
     <row r="28" spans="1:24" ht="15.75" customHeight="1">
       <c r="A28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B28" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="B28" t="s">
-        <v>94</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>27</v>
@@ -3514,13 +3476,13 @@
     </row>
     <row r="29" spans="1:24" ht="15.75" customHeight="1">
       <c r="A29" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="B29" t="s">
-        <v>94</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>49</v>
@@ -3588,13 +3550,13 @@
     </row>
     <row r="30" spans="1:24" ht="15.75" customHeight="1">
       <c r="A30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" t="s">
         <v>100</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>49</v>
@@ -3608,8 +3570,8 @@
       <c r="G30" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H30" s="1" t="s">
-        <v>103</v>
+      <c r="H30" s="1">
+        <v>500000</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>46</v>
@@ -3662,13 +3624,13 @@
     </row>
     <row r="31" spans="1:24" ht="15.75" customHeight="1">
       <c r="A31" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>27</v>
@@ -3736,13 +3698,13 @@
     </row>
     <row r="32" spans="1:24" ht="15.75" customHeight="1">
       <c r="A32" t="s">
+        <v>104</v>
+      </c>
+      <c r="B32" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="B32" t="s">
-        <v>107</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>27</v>
@@ -3762,17 +3724,17 @@
     </row>
     <row r="33" spans="1:24" ht="15.75" customHeight="1">
       <c r="A33" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33" t="s">
+        <v>105</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B33" t="s">
-        <v>107</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="E33" s="1" t="s">
         <v>33</v>
       </c>
@@ -3782,8 +3744,8 @@
       <c r="G33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H33" s="1" t="s">
-        <v>112</v>
+      <c r="H33" s="1">
+        <v>2000000</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>46</v>
@@ -3836,16 +3798,16 @@
     </row>
     <row r="34" spans="1:24" ht="15.75" customHeight="1">
       <c r="A34" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B34" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>33</v>
@@ -3856,50 +3818,50 @@
       <c r="G34" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H34" s="1" t="s">
+      <c r="H34" s="1">
+        <v>2000000</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="R34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="S34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U34" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V34" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L34" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M34" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="N34" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O34" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="P34" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q34" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="R34" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S34" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T34" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="U34" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="V34" s="1" t="s">
-        <v>115</v>
       </c>
       <c r="W34" s="1" t="s">
         <v>29</v>
@@ -3910,16 +3872,16 @@
     </row>
     <row r="35" spans="1:24" ht="15.75" customHeight="1">
       <c r="A35" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B35" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>33</v>
@@ -3984,16 +3946,16 @@
     </row>
     <row r="36" spans="1:24" ht="15.75" customHeight="1">
       <c r="A36" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B36" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>33</v>
@@ -4004,8 +3966,8 @@
       <c r="G36" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>120</v>
+      <c r="H36" s="1">
+        <v>500000</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>29</v>
@@ -4058,16 +4020,16 @@
     </row>
     <row r="37" spans="1:24" ht="15.75" customHeight="1">
       <c r="A37" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B37" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>33</v>
@@ -4132,16 +4094,16 @@
     </row>
     <row r="38" spans="1:24" ht="15.75" customHeight="1">
       <c r="A38" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B38" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>33</v>
@@ -4206,16 +4168,16 @@
     </row>
     <row r="39" spans="1:24" ht="15.75" customHeight="1">
       <c r="A39" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B39" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>33</v>
@@ -4230,7 +4192,7 @@
         <v>500000</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>29</v>
@@ -4280,16 +4242,16 @@
     </row>
     <row r="40" spans="1:24" ht="15.75" customHeight="1">
       <c r="A40" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B40" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>33</v>
@@ -4354,16 +4316,16 @@
     </row>
     <row r="41" spans="1:24" ht="15.75" customHeight="1">
       <c r="A41" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B41" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>33</v>
@@ -4428,16 +4390,16 @@
     </row>
     <row r="42" spans="1:24" ht="15.75" customHeight="1">
       <c r="A42" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B42" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>33</v>
@@ -4502,13 +4464,13 @@
     </row>
     <row r="43" spans="1:24" ht="15.75" customHeight="1">
       <c r="A43" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B43" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>49</v>
@@ -4576,13 +4538,13 @@
     </row>
     <row r="44" spans="1:24" ht="15.75" customHeight="1">
       <c r="A44" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B44" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>49</v>
@@ -4650,13 +4612,13 @@
     </row>
     <row r="45" spans="1:24" ht="15.75" customHeight="1">
       <c r="A45" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B45" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>49</v>
@@ -4724,13 +4686,13 @@
     </row>
     <row r="46" spans="1:24" ht="15.75" customHeight="1">
       <c r="A46" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B46" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>49</v>
@@ -4744,8 +4706,8 @@
       <c r="G46" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H46" s="1" t="s">
-        <v>103</v>
+      <c r="H46" s="1">
+        <v>500000</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>46</v>
@@ -4798,13 +4760,13 @@
     </row>
     <row r="47" spans="1:24" ht="15.75" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B47" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>27</v>
@@ -4872,13 +4834,13 @@
     </row>
     <row r="48" spans="1:24" ht="15.75" customHeight="1">
       <c r="A48" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B48" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>49</v>
@@ -4892,8 +4854,8 @@
       <c r="G48" s="9">
         <v>0.5</v>
       </c>
-      <c r="H48" s="1" t="s">
-        <v>148</v>
+      <c r="H48" s="1">
+        <v>100000</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>29</v>
@@ -4946,13 +4908,13 @@
     </row>
     <row r="49" spans="1:24" ht="15.75" customHeight="1">
       <c r="A49" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B49" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>49</v>
@@ -4966,8 +4928,8 @@
       <c r="G49" s="9">
         <v>0.5</v>
       </c>
-      <c r="H49" s="1" t="s">
-        <v>151</v>
+      <c r="H49" s="1">
+        <v>200000</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>29</v>
@@ -5020,13 +4982,13 @@
     </row>
     <row r="50" spans="1:24" ht="15.75" customHeight="1">
       <c r="A50" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B50" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>49</v>
@@ -5037,8 +4999,8 @@
       <c r="G50" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H50" s="1" t="s">
-        <v>151</v>
+      <c r="H50" s="1">
+        <v>200000</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>29</v>
@@ -5091,13 +5053,13 @@
     </row>
     <row r="51" spans="1:24" ht="15.75" customHeight="1">
       <c r="A51" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B51" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>27</v>
@@ -5165,13 +5127,13 @@
     </row>
     <row r="52" spans="1:24" ht="15.75" customHeight="1">
       <c r="A52" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B52" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>27</v>
@@ -5239,13 +5201,13 @@
     </row>
     <row r="53" spans="1:24" ht="15.75" customHeight="1">
       <c r="A53" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B53" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>49</v>
@@ -5259,8 +5221,8 @@
       <c r="G53" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H53" s="1" t="s">
-        <v>161</v>
+      <c r="H53" s="1">
+        <v>300000</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>29</v>
@@ -5313,13 +5275,13 @@
     </row>
     <row r="54" spans="1:24" ht="15.75" customHeight="1">
       <c r="A54" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B54" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>49</v>
@@ -5333,8 +5295,8 @@
       <c r="G54" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H54" s="1" t="s">
-        <v>103</v>
+      <c r="H54" s="1">
+        <v>500000</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>46</v>
@@ -5387,13 +5349,13 @@
     </row>
     <row r="55" spans="1:24" ht="15.75" customHeight="1">
       <c r="A55" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="B55" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>49</v>
@@ -5404,8 +5366,8 @@
       <c r="G55" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H55" s="1" t="s">
-        <v>167</v>
+      <c r="H55" s="1">
+        <v>199000</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>29</v>
@@ -5458,13 +5420,13 @@
     </row>
     <row r="56" spans="1:24" ht="15.75" customHeight="1">
       <c r="A56" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B56" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>49</v>
@@ -5478,8 +5440,8 @@
       <c r="G56" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H56" s="1" t="s">
-        <v>103</v>
+      <c r="H56" s="1">
+        <v>500000</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>29</v>
@@ -5532,13 +5494,13 @@
     </row>
     <row r="57" spans="1:24" ht="15.75" customHeight="1">
       <c r="A57" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="B57" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>27</v>
@@ -5606,13 +5568,13 @@
     </row>
     <row r="58" spans="1:24" ht="15.75" customHeight="1">
       <c r="A58" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="B58" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>89</v>
@@ -5680,16 +5642,16 @@
     </row>
     <row r="59" spans="1:24" ht="15.75" customHeight="1">
       <c r="A59" s="10" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B59" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>33</v>
@@ -5700,8 +5662,8 @@
       <c r="G59" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H59" s="1" t="s">
-        <v>112</v>
+      <c r="H59" s="1">
+        <v>2000000</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>46</v>
@@ -5709,13 +5671,13 @@
     </row>
     <row r="60" spans="1:24" ht="15.75" customHeight="1">
       <c r="A60" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="B60" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>49</v>
@@ -5729,8 +5691,8 @@
       <c r="G60" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H60" s="1" t="s">
-        <v>103</v>
+      <c r="H60" s="1">
+        <v>500000</v>
       </c>
       <c r="I60" s="1" t="s">
         <v>46</v>
@@ -5783,13 +5745,13 @@
     </row>
     <row r="61" spans="1:24" ht="15.75" customHeight="1">
       <c r="A61" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="B61" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>49</v>
@@ -5857,13 +5819,13 @@
     </row>
     <row r="62" spans="1:24" ht="15.75" customHeight="1">
       <c r="A62" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="B62" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>49</v>
@@ -5931,13 +5893,13 @@
     </row>
     <row r="63" spans="1:24" ht="15.75" customHeight="1">
       <c r="A63" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B63" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>49</v>
@@ -6005,13 +5967,13 @@
     </row>
     <row r="64" spans="1:24" ht="15.75" customHeight="1">
       <c r="A64" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="B64" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>49</v>
@@ -6025,8 +5987,8 @@
       <c r="G64" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H64" s="1" t="s">
-        <v>187</v>
+      <c r="H64" s="1">
+        <v>100000</v>
       </c>
       <c r="I64" s="1" t="s">
         <v>46</v>
@@ -6079,13 +6041,13 @@
     </row>
     <row r="65" spans="1:24" ht="15.75" customHeight="1">
       <c r="A65" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B65" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>49</v>
@@ -6153,13 +6115,13 @@
     </row>
     <row r="66" spans="1:24" ht="15.75" customHeight="1">
       <c r="A66" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B66" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>49</v>
@@ -6227,13 +6189,13 @@
     </row>
     <row r="67" spans="1:24" ht="15.75" customHeight="1">
       <c r="A67" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B67" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>49</v>
@@ -6247,8 +6209,8 @@
       <c r="G67" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H67" s="1" t="s">
-        <v>103</v>
+      <c r="H67" s="1">
+        <v>500000</v>
       </c>
       <c r="I67" s="1" t="s">
         <v>46</v>
@@ -6301,13 +6263,13 @@
     </row>
     <row r="68" spans="1:24" ht="15.75" customHeight="1">
       <c r="A68" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="B68" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>49</v>
@@ -6375,13 +6337,13 @@
     </row>
     <row r="69" spans="1:24" ht="15.75" customHeight="1">
       <c r="A69" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B69" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>49</v>
@@ -6449,13 +6411,13 @@
     </row>
     <row r="70" spans="1:24" ht="15.75" customHeight="1">
       <c r="A70" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="B70" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>49</v>
@@ -6523,13 +6485,13 @@
     </row>
     <row r="71" spans="1:24" ht="15.75" customHeight="1">
       <c r="A71" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B71" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>27</v>
@@ -6597,13 +6559,13 @@
     </row>
     <row r="72" spans="1:24" ht="15.75" customHeight="1">
       <c r="A72" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B72" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>27</v>
@@ -6671,13 +6633,13 @@
     </row>
     <row r="73" spans="1:24" ht="15.75" customHeight="1">
       <c r="A73" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="B73" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>27</v>
@@ -6745,13 +6707,13 @@
     </row>
     <row r="74" spans="1:24" ht="15.75" customHeight="1">
       <c r="A74" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B74" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>27</v>
@@ -6819,13 +6781,13 @@
     </row>
     <row r="75" spans="1:24" ht="15.75" customHeight="1">
       <c r="A75" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="B75" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>27</v>
@@ -6893,13 +6855,13 @@
     </row>
     <row r="76" spans="1:24" ht="15.75" customHeight="1">
       <c r="A76" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="B76" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>27</v>
@@ -6967,13 +6929,13 @@
     </row>
     <row r="77" spans="1:24" ht="15.75" customHeight="1">
       <c r="A77" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="B77" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>27</v>
@@ -7041,19 +7003,19 @@
     </row>
     <row r="78" spans="1:24" ht="15.75" customHeight="1">
       <c r="A78" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="B78" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>49</v>
       </c>
       <c r="E78" s="11">
-        <v>2.0799999999999999E-2</v>
+        <v>2.08</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>33</v>
@@ -7115,13 +7077,13 @@
     </row>
     <row r="79" spans="1:24" ht="15.75" customHeight="1">
       <c r="A79" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B79" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>27</v>
@@ -7132,8 +7094,8 @@
       <c r="F79" s="7">
         <v>20000</v>
       </c>
-      <c r="G79" s="1" t="s">
-        <v>148</v>
+      <c r="G79" s="1">
+        <v>100000</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>33</v>
@@ -7186,13 +7148,13 @@
     </row>
     <row r="80" spans="1:24" ht="15.75" customHeight="1">
       <c r="A80" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B80" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>49</v>
@@ -7260,13 +7222,13 @@
     </row>
     <row r="81" spans="1:24" ht="15.75" customHeight="1">
       <c r="A81" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="B81" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>27</v>
@@ -7334,13 +7296,13 @@
     </row>
     <row r="82" spans="1:24" ht="15.75" customHeight="1">
       <c r="A82" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="B82" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>49</v>
@@ -7354,8 +7316,8 @@
       <c r="G82" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H82" s="1" t="s">
-        <v>103</v>
+      <c r="H82" s="1">
+        <v>500000</v>
       </c>
       <c r="I82" s="1" t="s">
         <v>46</v>
@@ -7408,13 +7370,13 @@
     </row>
     <row r="83" spans="1:24" ht="15.75" customHeight="1">
       <c r="A83" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="B83" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>49</v>
@@ -7428,8 +7390,8 @@
       <c r="G83" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H83" s="1" t="s">
-        <v>103</v>
+      <c r="H83" s="1">
+        <v>500000</v>
       </c>
       <c r="I83" s="1" t="s">
         <v>46</v>
@@ -7479,27 +7441,29 @@
     </row>
     <row r="84" spans="1:24" ht="15.75" customHeight="1">
       <c r="A84" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="B84" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="D84" s="1"/>
+        <v>216</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="F84" s="7"/>
       <c r="T84" s="1"/>
     </row>
     <row r="85" spans="1:24" ht="15.75" customHeight="1">
       <c r="A85" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="B85" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>27</v>
@@ -7567,13 +7531,13 @@
     </row>
     <row r="86" spans="1:24" ht="15.75" customHeight="1">
       <c r="A86" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="B86" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>49</v>
@@ -7641,13 +7605,13 @@
     </row>
     <row r="87" spans="1:24" ht="15.75" customHeight="1">
       <c r="A87" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="B87" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>49</v>
@@ -7715,13 +7679,13 @@
     </row>
     <row r="88" spans="1:24" ht="15.75" customHeight="1">
       <c r="A88" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B88" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>49</v>
@@ -7789,13 +7753,13 @@
     </row>
     <row r="89" spans="1:24" ht="15.75" customHeight="1">
       <c r="A89" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B89" t="s">
+        <v>218</v>
+      </c>
+      <c r="C89" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>236</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>49</v>
@@ -7863,13 +7827,13 @@
     </row>
     <row r="90" spans="1:24" ht="15.75" customHeight="1">
       <c r="A90" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="B90" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>49</v>
@@ -7937,13 +7901,13 @@
     </row>
     <row r="91" spans="1:24" ht="15.75" customHeight="1">
       <c r="A91" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="B91" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>49</v>
@@ -7957,8 +7921,8 @@
       <c r="G91" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H91" s="1" t="s">
-        <v>241</v>
+      <c r="H91" s="1">
+        <v>2500000</v>
       </c>
       <c r="I91" s="1" t="s">
         <v>29</v>
@@ -8011,13 +7975,13 @@
     </row>
     <row r="92" spans="1:24" ht="15.75" customHeight="1">
       <c r="A92" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="B92" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>49</v>
@@ -8085,13 +8049,13 @@
     </row>
     <row r="93" spans="1:24" ht="15.75" customHeight="1">
       <c r="A93" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="B93" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>49</v>
@@ -8156,13 +8120,13 @@
     </row>
     <row r="94" spans="1:24" ht="15.75" customHeight="1">
       <c r="A94" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="B94" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>49</v>
@@ -8176,8 +8140,8 @@
       <c r="G94" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H94" s="1" t="s">
-        <v>103</v>
+      <c r="H94" s="1">
+        <v>500000</v>
       </c>
       <c r="I94" s="1" t="s">
         <v>46</v>
@@ -8230,13 +8194,13 @@
     </row>
     <row r="95" spans="1:24" ht="15.75" customHeight="1">
       <c r="A95" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="B95" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>49</v>
@@ -8250,8 +8214,8 @@
       <c r="G95" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H95" s="1" t="s">
-        <v>251</v>
+      <c r="H95" s="1">
+        <v>12000000</v>
       </c>
       <c r="I95" s="1" t="s">
         <v>29</v>
@@ -8298,13 +8262,13 @@
     </row>
     <row r="96" spans="1:24" ht="15.75" customHeight="1">
       <c r="A96" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="B96" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>49</v>
@@ -8318,8 +8282,8 @@
       <c r="G96" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H96" s="1" t="s">
-        <v>103</v>
+      <c r="H96" s="1">
+        <v>500000</v>
       </c>
       <c r="I96" s="1" t="s">
         <v>29</v>
@@ -8372,13 +8336,13 @@
     </row>
     <row r="97" spans="1:24" ht="15.75" customHeight="1">
       <c r="A97" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="B97" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>27</v>
@@ -8446,13 +8410,13 @@
     </row>
     <row r="98" spans="1:24" ht="15.75" customHeight="1">
       <c r="A98" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="B98" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>89</v>
@@ -8517,16 +8481,16 @@
     </row>
     <row r="99" spans="1:24" ht="15.75" customHeight="1">
       <c r="A99" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="B99" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>33</v>
@@ -8591,16 +8555,16 @@
     </row>
     <row r="100" spans="1:24" ht="15.75" customHeight="1">
       <c r="A100" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="B100" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>33</v>
@@ -8665,13 +8629,13 @@
     </row>
     <row r="101" spans="1:24" ht="15.75" customHeight="1">
       <c r="A101" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="B101" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>27</v>
@@ -8739,13 +8703,13 @@
     </row>
     <row r="102" spans="1:24" ht="15.75" customHeight="1">
       <c r="A102" s="1" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="B102" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>49</v>
@@ -8813,13 +8777,13 @@
     </row>
     <row r="103" spans="1:24" ht="15.75" customHeight="1">
       <c r="A103" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="B103" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>27</v>
@@ -8887,13 +8851,13 @@
     </row>
     <row r="104" spans="1:24" ht="15.75" customHeight="1">
       <c r="A104" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="B104" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>49</v>
@@ -8961,13 +8925,13 @@
     </row>
     <row r="105" spans="1:24" ht="15.75" customHeight="1">
       <c r="A105" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="B105" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>49</v>
@@ -9035,13 +8999,13 @@
     </row>
     <row r="106" spans="1:24" ht="15.75" customHeight="1">
       <c r="A106" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="B106" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>49</v>
@@ -9055,8 +9019,8 @@
       <c r="G106" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H106" s="1" t="s">
-        <v>275</v>
+      <c r="H106" s="1">
+        <v>200000</v>
       </c>
       <c r="I106" s="1" t="s">
         <v>46</v>
@@ -9109,13 +9073,13 @@
     </row>
     <row r="107" spans="1:24" ht="15.75" customHeight="1">
       <c r="A107" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="B107" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>49</v>
@@ -9129,8 +9093,8 @@
       <c r="G107" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H107" s="1" t="s">
-        <v>275</v>
+      <c r="H107" s="1">
+        <v>200000</v>
       </c>
       <c r="I107" s="1" t="s">
         <v>46</v>
@@ -9183,13 +9147,13 @@
     </row>
     <row r="108" spans="1:24" ht="15.75" customHeight="1">
       <c r="A108" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="B108" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>49</v>
@@ -9203,8 +9167,8 @@
       <c r="G108" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H108" s="1" t="s">
-        <v>278</v>
+      <c r="H108" s="1">
+        <v>500000</v>
       </c>
       <c r="I108" s="1" t="s">
         <v>46</v>
@@ -9257,13 +9221,13 @@
     </row>
     <row r="109" spans="1:24" ht="15.75" customHeight="1">
       <c r="A109" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="B109" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>49</v>
@@ -9277,8 +9241,8 @@
       <c r="G109" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H109" s="1" t="s">
-        <v>278</v>
+      <c r="H109" s="1">
+        <v>500000</v>
       </c>
       <c r="I109" s="1" t="s">
         <v>46</v>
@@ -9331,13 +9295,13 @@
     </row>
     <row r="110" spans="1:24" ht="15.75" customHeight="1">
       <c r="A110" s="1" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="C110" s="15" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>27</v>
@@ -9349,7 +9313,7 @@
         <v>33</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="H110" s="1" t="s">
         <v>33</v>
@@ -9405,13 +9369,13 @@
     </row>
     <row r="111" spans="1:24" ht="15.75" customHeight="1">
       <c r="A111" s="1" t="s">
-        <v>284</v>
+        <v>271</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="C111" s="15" t="s">
-        <v>282</v>
+        <v>269</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>27</v>
@@ -9423,7 +9387,7 @@
         <v>33</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>285</v>
+        <v>272</v>
       </c>
       <c r="H111" s="1" t="s">
         <v>33</v>
@@ -9479,13 +9443,13 @@
     </row>
     <row r="112" spans="1:24" ht="15.75" customHeight="1">
       <c r="A112" s="1" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="C112" s="15" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>49</v>
@@ -9499,8 +9463,8 @@
       <c r="G112" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H112" s="1" t="s">
-        <v>187</v>
+      <c r="H112" s="1">
+        <v>100000</v>
       </c>
       <c r="I112" s="1" t="s">
         <v>46</v>
@@ -9553,13 +9517,13 @@
     </row>
     <row r="113" spans="1:24" ht="15.75" customHeight="1">
       <c r="A113" s="1" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="C113" s="15" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>49</v>
@@ -9627,13 +9591,13 @@
     </row>
     <row r="114" spans="1:24" ht="15.75" customHeight="1">
       <c r="A114" s="1" t="s">
-        <v>289</v>
+        <v>276</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="C114" s="15" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>49</v>
@@ -9701,13 +9665,13 @@
     </row>
     <row r="115" spans="1:24" ht="15.75" customHeight="1">
       <c r="A115" s="1" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="C115" s="15" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>49</v>
@@ -9775,13 +9739,13 @@
     </row>
     <row r="116" spans="1:24" ht="15.75" customHeight="1">
       <c r="A116" s="1" t="s">
-        <v>291</v>
+        <v>278</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="C116" s="15" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>49</v>
@@ -9849,13 +9813,13 @@
     </row>
     <row r="117" spans="1:24" ht="15.75" customHeight="1">
       <c r="A117" s="1" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="C117" s="15" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>49</v>
@@ -9923,13 +9887,13 @@
     </row>
     <row r="118" spans="1:24" ht="15.75" customHeight="1">
       <c r="A118" s="1" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="C118" s="15" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>27</v>
@@ -9997,13 +9961,13 @@
     </row>
     <row r="119" spans="1:24" ht="15.75" customHeight="1">
       <c r="A119" s="1" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="C119" s="15" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>27</v>
@@ -10071,13 +10035,13 @@
     </row>
     <row r="120" spans="1:24" ht="15.75" customHeight="1">
       <c r="A120" s="1" t="s">
-        <v>298</v>
+        <v>285</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="C120" s="15" t="s">
-        <v>299</v>
+        <v>286</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>49</v>
@@ -10145,13 +10109,13 @@
     </row>
     <row r="121" spans="1:24" ht="15.75" customHeight="1">
       <c r="A121" s="1" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="C121" s="15" t="s">
-        <v>301</v>
+        <v>288</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>49</v>
@@ -10219,13 +10183,13 @@
     </row>
     <row r="122" spans="1:24" ht="15.75" customHeight="1">
       <c r="A122" s="1" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="C122" s="15" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>49</v>
@@ -10293,13 +10257,13 @@
     </row>
     <row r="123" spans="1:24" ht="15.75" customHeight="1">
       <c r="A123" s="1" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>89</v>
@@ -10307,13 +10271,13 @@
     </row>
     <row r="124" spans="1:24" ht="15.75" customHeight="1">
       <c r="A124" s="1" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>27</v>
@@ -10381,13 +10345,13 @@
     </row>
     <row r="125" spans="1:24" ht="15.75" customHeight="1">
       <c r="A125" s="1" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="C125" s="15" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>49</v>
@@ -10455,13 +10419,13 @@
     </row>
     <row r="126" spans="1:24" ht="15.75" customHeight="1">
       <c r="A126" s="1" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="C126" s="15" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="D126" s="1" t="s">
         <v>49</v>
@@ -10529,13 +10493,13 @@
     </row>
     <row r="127" spans="1:24" ht="15.75" customHeight="1">
       <c r="A127" s="1" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="C127" s="15" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>49</v>
@@ -10603,13 +10567,13 @@
     </row>
     <row r="128" spans="1:24" ht="15.75" customHeight="1">
       <c r="A128" s="1" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="C128" s="15" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>49</v>
@@ -10677,16 +10641,16 @@
     </row>
     <row r="129" spans="1:24" ht="15.75" customHeight="1">
       <c r="A129" s="1" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="C129" s="15" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="E129" s="1" t="s">
         <v>33</v>
@@ -10751,16 +10715,16 @@
     </row>
     <row r="130" spans="1:24" ht="15.75" customHeight="1">
       <c r="A130" s="1" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="C130" s="15" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="E130" s="1" t="s">
         <v>33</v>
@@ -10825,13 +10789,13 @@
     </row>
     <row r="131" spans="1:24" ht="15.75" customHeight="1">
       <c r="A131" s="1" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="C131" s="15" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>89</v>

</xml_diff>